<commit_message>
done unit test for labelMutationGroup
</commit_message>
<xml_diff>
--- a/fluidigmLogicalTable.xlsx
+++ b/fluidigmLogicalTable.xlsx
@@ -1,30 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Geyi\OneDrive\Documents\Documents\BCCRC\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20500" windowHeight="7540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="130407"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>Outcome</t>
   </si>
@@ -74,80 +72,93 @@
     <t>T1, T2, T2, N</t>
   </si>
   <si>
+    <t>T1,N</t>
+  </si>
+  <si>
+    <t>T1,T1,T2</t>
+  </si>
+  <si>
+    <t>T1,T1,T2,T2</t>
+  </si>
+  <si>
+    <t>somatic, somatic, somatic, somatic</t>
+  </si>
+  <si>
+    <t>T1,T1,T2,N</t>
+  </si>
+  <si>
+    <t>T1, T1, T2, T2, N</t>
+  </si>
+  <si>
+    <t>T1,T1,N</t>
+  </si>
+  <si>
+    <t>T2, N</t>
+  </si>
+  <si>
+    <t>T2,T2, N</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>artifact, artifact, normal</t>
+  </si>
+  <si>
+    <t>artifact, germline, germline, normal</t>
+  </si>
+  <si>
+    <t>T2, T1, T2,N</t>
+  </si>
+  <si>
+    <t>germline, artifact, germline, normal</t>
+  </si>
+  <si>
+    <t>germline, germline, artifact, normal</t>
+  </si>
+  <si>
+    <t>germline,germline, germline, germline,normal</t>
+  </si>
+  <si>
+    <t>germline, germline, normal</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Covered</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>artifact, normal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>somatic, somatic, artifact</t>
-  </si>
-  <si>
-    <t>T1,N</t>
-  </si>
-  <si>
-    <t>T1,T1,T2</t>
-  </si>
-  <si>
-    <t>T1,T1,T2,T2</t>
-  </si>
-  <si>
-    <t>somatic, somatic, somatic, somatic</t>
-  </si>
-  <si>
-    <t>T1,T1,T2,N</t>
-  </si>
-  <si>
-    <t>T1, T1, T2, T2, N</t>
-  </si>
-  <si>
-    <t>T1,T1,N</t>
-  </si>
-  <si>
-    <t>T2, N</t>
-  </si>
-  <si>
-    <t>T2,T2, N</t>
-  </si>
-  <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>artifact, artifact, normal</t>
-  </si>
-  <si>
-    <t>artifact, germline, germline, normal</t>
-  </si>
-  <si>
-    <t>T2, T1, T2,N</t>
-  </si>
-  <si>
-    <t>germline, artifact, germline, normal</t>
-  </si>
-  <si>
-    <t>germline, germline, artifact, normal</t>
-  </si>
-  <si>
-    <t>germline,germline, germline, germline,normal</t>
-  </si>
-  <si>
-    <t>germline, germline, normal</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Covered</t>
-  </si>
-  <si>
-    <t>Case</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>artifact, normal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="6">
@@ -206,7 +217,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -261,7 +272,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -313,7 +324,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -507,34 +518,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="B1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="8" max="8" width="9.28515625" customWidth="1"/>
-    <col min="9" max="9" width="27.140625" customWidth="1"/>
-    <col min="10" max="10" width="47.42578125" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="27.1640625" customWidth="1"/>
+    <col min="10" max="10" width="47.5" customWidth="1"/>
+    <col min="11" max="11" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12">
       <c r="B1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -558,12 +569,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12">
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -587,15 +598,15 @@
         <v>8</v>
       </c>
       <c r="L2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12">
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -619,15 +630,15 @@
         <v>8</v>
       </c>
       <c r="L3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12">
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -651,12 +662,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12">
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -680,12 +691,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12">
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -706,15 +717,15 @@
         <v>14</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -735,15 +746,15 @@
         <v>15</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
@@ -761,18 +772,18 @@
         <v>1</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
@@ -790,18 +801,18 @@
         <v>0</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12">
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
@@ -819,18 +830,18 @@
         <v>0</v>
       </c>
       <c r="I10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="2:12">
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="3">
         <v>0</v>
@@ -848,18 +859,18 @@
         <v>1</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12">
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="3">
         <v>0</v>
@@ -877,18 +888,18 @@
         <v>1</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12">
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="3">
         <v>0</v>
@@ -906,18 +917,18 @@
         <v>1</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12">
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="5">
         <v>0</v>
@@ -935,18 +946,18 @@
         <v>1</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12">
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="5">
         <v>0</v>
@@ -964,24 +975,30 @@
         <v>1</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12">
       <c r="D16" s="4"/>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:9">
       <c r="H18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" t="s">
         <v>29</v>
       </c>
-      <c r="I18" t="s">
-        <v>30</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>